<commit_message>
created data frame and excel doc with population and per capita gdp from 1960 and 2019
</commit_message>
<xml_diff>
--- a/Ken_Jpn_USA.xlsx
+++ b/Ken_Jpn_USA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Econ1540\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D3B6CB-5725-45FC-9EA6-AFEB15077C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE57D7BC-5D7A-4200-B548-A1A7B3AB457F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1200" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,9 +534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E146" sqref="E146:E211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6709,10 +6709,6 @@
       <c r="E72">
         <v>84.274266913120172</v>
       </c>
-      <c r="F72">
-        <f t="shared" si="0"/>
-        <v>1.0050657028005014</v>
-      </c>
       <c r="G72">
         <v>2.2900006771087651</v>
       </c>
@@ -6748,10 +6744,6 @@
       <c r="E73">
         <v>85.64072436572404</v>
       </c>
-      <c r="F73">
-        <f t="shared" si="0"/>
-        <v>0.98342167094784905</v>
-      </c>
       <c r="G73">
         <v>2.3225193023681641</v>
       </c>
@@ -6805,10 +6797,6 @@
       <c r="E74">
         <v>86.943150343431171</v>
       </c>
-      <c r="F74">
-        <f t="shared" si="0"/>
-        <v>0.96067552280995927</v>
-      </c>
       <c r="G74">
         <v>2.3554997444152832</v>
       </c>
@@ -6862,10 +6850,6 @@
       <c r="E75">
         <v>88.145992263606601</v>
       </c>
-      <c r="F75">
-        <f t="shared" si="0"/>
-        <v>0.93642418839336949</v>
-      </c>
       <c r="G75">
         <v>2.3889484405517578</v>
       </c>
@@ -6919,10 +6903,6 @@
       <c r="E76">
         <v>89.250868942593883</v>
       </c>
-      <c r="F76">
-        <f t="shared" si="0"/>
-        <v>0.91115125972750743</v>
-      </c>
       <c r="G76">
         <v>2.4228720664978032</v>
       </c>
@@ -6982,10 +6962,6 @@
       <c r="E77">
         <v>90.317983469718982</v>
       </c>
-      <c r="F77">
-        <f t="shared" ref="F77:F140" si="3">(E77-E67)/E67</f>
-        <v>0.88640606619492768</v>
-      </c>
       <c r="G77">
         <v>2.4572772979736328</v>
       </c>
@@ -7020,14 +6996,14 @@
         <v>3950.9915970349371</v>
       </c>
       <c r="X77">
-        <f t="shared" ref="X77:X140" si="4">(W77-W67)/W67</f>
+        <f t="shared" ref="X77:X140" si="3">(W77-W67)/W67</f>
         <v>0.17769599040006917</v>
       </c>
       <c r="Y77">
         <v>3785.075719329096</v>
       </c>
       <c r="Z77">
-        <f t="shared" ref="Z77:Z140" si="5">(Y77-Y67)/Y67</f>
+        <f t="shared" ref="Z77:Z140" si="4">(Y77-Y67)/Y67</f>
         <v>6.9765819624455563E-2</v>
       </c>
       <c r="AA77">
@@ -7051,10 +7027,6 @@
       <c r="E78">
         <v>91.274458421060984</v>
       </c>
-      <c r="F78">
-        <f t="shared" si="3"/>
-        <v>0.8607870331040206</v>
-      </c>
       <c r="G78">
         <v>2.4841210842132568</v>
       </c>
@@ -7089,14 +7061,14 @@
         <v>4172.1056918605746</v>
       </c>
       <c r="X78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.16371267838763354</v>
       </c>
       <c r="Y78">
         <v>4000.8286553222501</v>
       </c>
       <c r="Z78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.4718835778188053E-2</v>
       </c>
       <c r="AA78">
@@ -7120,10 +7092,6 @@
       <c r="E79">
         <v>92.075718806307179</v>
       </c>
-      <c r="F79">
-        <f t="shared" si="3"/>
-        <v>0.83340551686991071</v>
-      </c>
       <c r="G79">
         <v>2.5112578868865971</v>
       </c>
@@ -7158,14 +7126,14 @@
         <v>4410.6789799199596</v>
       </c>
       <c r="X79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.13077166677193519</v>
       </c>
       <c r="Y79">
         <v>4244.8076845556716</v>
       </c>
       <c r="Z79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.9419156753421289E-2</v>
       </c>
       <c r="AA79">
@@ -7189,10 +7157,6 @@
       <c r="E80">
         <v>92.906102541506385</v>
       </c>
-      <c r="F80">
-        <f t="shared" si="3"/>
-        <v>0.80777321664148094</v>
-      </c>
       <c r="G80">
         <v>2.5386912822723389</v>
       </c>
@@ -7227,14 +7191,14 @@
         <v>4760.9614750806031</v>
       </c>
       <c r="X80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.18208108624301339</v>
       </c>
       <c r="Y80">
         <v>4512.6092477369602</v>
       </c>
       <c r="Z80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.3215977127920638E-2</v>
       </c>
       <c r="AA80">
@@ -7258,10 +7222,6 @@
       <c r="E81">
         <v>93.818976861187949</v>
       </c>
-      <c r="F81">
-        <f t="shared" si="3"/>
-        <v>0.78451373384294054</v>
-      </c>
       <c r="G81">
         <v>2.5643172264099121</v>
       </c>
@@ -7296,14 +7256,14 @@
         <v>5182.9829371243359</v>
       </c>
       <c r="X81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.25265806838596494</v>
       </c>
       <c r="Y81">
         <v>4889.3762924818966</v>
       </c>
       <c r="Z81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.1540617057770059</v>
       </c>
       <c r="AA81">
@@ -7328,7 +7288,7 @@
         <v>94.618503348359994</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F77:F140" si="5">(E82-E72)/E72</f>
         <v>0.12274489964895069</v>
       </c>
       <c r="G82">
@@ -7377,14 +7337,14 @@
         <v>5821.0912031885</v>
       </c>
       <c r="X82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0217899757138105</v>
       </c>
       <c r="Y82">
         <v>5473.6264622914987</v>
       </c>
       <c r="Z82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.95143272597171402</v>
       </c>
       <c r="AA82">
@@ -7415,7 +7375,7 @@
         <v>95.4749262431326</v>
       </c>
       <c r="F83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.11483090492570028</v>
       </c>
       <c r="G83">
@@ -7464,14 +7424,14 @@
         <v>6398.0895198014177</v>
       </c>
       <c r="X83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0293752348692322</v>
       </c>
       <c r="Y83">
         <v>6018.1743271189926</v>
       </c>
       <c r="Z83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.97253419314361989</v>
       </c>
       <c r="AA83">
@@ -7502,7 +7462,7 @@
         <v>96.368367094576271</v>
       </c>
       <c r="F84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10840666244453845</v>
       </c>
       <c r="G84">
@@ -7551,14 +7511,14 @@
         <v>6959.574964487977</v>
       </c>
       <c r="X84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.0486752422286378</v>
       </c>
       <c r="Y84">
         <v>6534.113127412732</v>
       </c>
       <c r="Z84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.97362206554668707</v>
       </c>
       <c r="AA84">
@@ -7589,7 +7549,7 @@
         <v>97.354042117025031</v>
       </c>
       <c r="F85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10446362468620388</v>
       </c>
       <c r="G85">
@@ -7638,14 +7598,14 @@
         <v>7473.350455499638</v>
       </c>
       <c r="X85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.1259682924049756</v>
       </c>
       <c r="Y85">
         <v>7003.3975752175465</v>
       </c>
       <c r="Z85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.052852733119785</v>
       </c>
       <c r="AA85">
@@ -7676,7 +7636,7 @@
         <v>98.374042183649195</v>
       </c>
       <c r="F86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10221943325754433</v>
       </c>
       <c r="G86">
@@ -7731,14 +7691,14 @@
         <v>8251.8598858076057</v>
       </c>
       <c r="X86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.23653988611034</v>
       </c>
       <c r="Y86">
         <v>7711.3076088082726</v>
       </c>
       <c r="Z86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1736002528761076</v>
       </c>
       <c r="AA86">
@@ -7769,7 +7729,7 @@
         <v>99.43622354058995</v>
       </c>
       <c r="F87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10095708208463325</v>
       </c>
       <c r="G87">
@@ -7824,14 +7784,14 @@
         <v>8700.6258302523129</v>
       </c>
       <c r="X87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.2021372651821856</v>
       </c>
       <c r="Y87">
         <v>8102.6351244233892</v>
       </c>
       <c r="Z87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1406797975126319</v>
       </c>
       <c r="AA87">
@@ -7862,7 +7822,7 @@
         <v>100.3490825160408</v>
       </c>
       <c r="F88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.9421286655215046E-2</v>
       </c>
       <c r="G88">
@@ -7917,14 +7877,14 @@
         <v>9497.3464241454858</v>
       </c>
       <c r="X88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.2763916174688492</v>
       </c>
       <c r="Y88">
         <v>8851.9138912705912</v>
       </c>
       <c r="Z88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2125201186746666</v>
       </c>
       <c r="AA88">
@@ -7955,7 +7915,7 @@
         <v>101.38985099897759</v>
       </c>
       <c r="F89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10115731175842199</v>
       </c>
       <c r="G89">
@@ -8010,14 +7970,14 @@
         <v>10390.77742614124</v>
       </c>
       <c r="X89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.3558226462289034</v>
       </c>
       <c r="Y89">
         <v>9667.9739425781845</v>
       </c>
       <c r="Z89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2775999906318929</v>
       </c>
       <c r="AA89">
@@ -8048,7 +8008,7 @@
         <v>102.5315998644439</v>
       </c>
       <c r="F90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10360457558358202</v>
       </c>
       <c r="G90">
@@ -8103,14 +8063,14 @@
         <v>11572.95410945294</v>
       </c>
       <c r="X90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.4308018810962988</v>
       </c>
       <c r="Y90">
         <v>10765.293348190229</v>
       </c>
       <c r="Z90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3856028202727597</v>
       </c>
       <c r="AA90">
@@ -8141,7 +8101,7 @@
         <v>103.7495405076719</v>
       </c>
       <c r="F91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10584813412724531</v>
       </c>
       <c r="G91">
@@ -8196,14 +8156,14 @@
         <v>12823.37486498671</v>
       </c>
       <c r="X91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.4741302490379176</v>
       </c>
       <c r="Y91">
         <v>11935.014304072371</v>
       </c>
       <c r="Z91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4410095664807254</v>
       </c>
       <c r="AA91">
@@ -8234,7 +8194,7 @@
         <v>104.92925099999999</v>
       </c>
       <c r="F92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10897178973206316</v>
       </c>
       <c r="G92">
@@ -8289,14 +8249,14 @@
         <v>14034.253899324989</v>
       </c>
       <c r="X92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.4109318011780563</v>
       </c>
       <c r="Y92">
         <v>13023.325116463469</v>
       </c>
       <c r="Z92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3792864212022495</v>
       </c>
       <c r="AA92">
@@ -8327,7 +8287,7 @@
         <v>106.427103</v>
       </c>
       <c r="F93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.11471259720041083</v>
       </c>
       <c r="G93">
@@ -8382,14 +8342,14 @@
         <v>14751.318797054921</v>
       </c>
       <c r="X93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.3055818071005623</v>
       </c>
       <c r="Y93">
         <v>13613.444875972989</v>
       </c>
       <c r="Z93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2620555896209786</v>
       </c>
       <c r="AA93">
@@ -8420,7 +8380,7 @@
         <v>107.976027</v>
       </c>
       <c r="F94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.12045093483873116</v>
       </c>
       <c r="G94">
@@ -8475,14 +8435,14 @@
         <v>15883.769968680181</v>
       </c>
       <c r="X94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.2822902332008668</v>
       </c>
       <c r="Y94">
         <v>14635.70358075872</v>
       </c>
       <c r="Z94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2398913663366462</v>
       </c>
       <c r="AA94">
@@ -8513,7 +8473,7 @@
         <v>109.52851200000001</v>
       </c>
       <c r="F95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.1250535634497906</v>
       </c>
       <c r="G95">
@@ -8568,14 +8528,14 @@
         <v>16877.87925029056</v>
       </c>
       <c r="X95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.2584086415845961</v>
       </c>
       <c r="Y95">
         <v>15587.0863561079</v>
       </c>
       <c r="Z95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2256463650250098</v>
       </c>
       <c r="AA95">
@@ -8606,7 +8566,7 @@
         <v>111.022689</v>
       </c>
       <c r="F96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.12857707720028144</v>
       </c>
       <c r="G96">
@@ -8661,14 +8621,14 @@
         <v>16179.93822866243</v>
       </c>
       <c r="X96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.96076259807687059</v>
       </c>
       <c r="Y96">
         <v>15280.525226694879</v>
       </c>
       <c r="Z96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.98157381366042729</v>
       </c>
       <c r="AA96">
@@ -8699,7 +8659,7 @@
         <v>112.413359</v>
       </c>
       <c r="F97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.130507123031606</v>
       </c>
       <c r="G97">
@@ -8754,14 +8714,14 @@
         <v>16556.249555713392</v>
       </c>
       <c r="X97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.90288030754602289</v>
       </c>
       <c r="Y97">
         <v>15796.55559442895</v>
       </c>
       <c r="Z97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.94955781074408008</v>
       </c>
       <c r="AA97">
@@ -8792,7 +8752,7 @@
         <v>113.679191</v>
       </c>
       <c r="F98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.13283737279639193</v>
       </c>
       <c r="G98">
@@ -8847,14 +8807,14 @@
         <v>17407.624100702829</v>
       </c>
       <c r="X98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.83289345500199152</v>
       </c>
       <c r="Y98">
         <v>16670.612566199561</v>
       </c>
       <c r="Z98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.88327776015076953</v>
       </c>
       <c r="AA98">
@@ -8885,7 +8845,7 @@
         <v>114.827832</v>
       </c>
       <c r="F99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.13253773300404509</v>
       </c>
       <c r="G99">
@@ -8940,14 +8900,14 @@
         <v>18377.334686594098</v>
       </c>
       <c r="X99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.76861979935785985</v>
       </c>
       <c r="Y99">
         <v>17632.516348475521</v>
       </c>
       <c r="Z99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.82380677204984387</v>
       </c>
       <c r="AA99">
@@ -8978,7 +8938,7 @@
         <v>115.879211</v>
       </c>
       <c r="F100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.13018046293243105</v>
       </c>
       <c r="G100">
@@ -9033,14 +8993,14 @@
         <v>19735.200820447419</v>
       </c>
       <c r="X100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.70528636282480806</v>
       </c>
       <c r="Y100">
         <v>18790.568482555511</v>
       </c>
       <c r="Z100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.74547667906461867</v>
       </c>
       <c r="AA100">
@@ -9071,7 +9031,7 @@
         <v>116.867356</v>
       </c>
       <c r="F101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.12643733580061584</v>
       </c>
       <c r="G101">
@@ -9126,14 +9086,14 @@
         <v>20628.277497781331</v>
       </c>
       <c r="X101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.60864653142951775</v>
       </c>
       <c r="Y101">
         <v>19873.618514994039</v>
       </c>
       <c r="Z101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.66515246724194721</v>
       </c>
       <c r="AA101">
@@ -9164,7 +9124,7 @@
         <v>117.81694</v>
       </c>
       <c r="F102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.12282265314178226</v>
       </c>
       <c r="G102">
@@ -9219,14 +9179,14 @@
         <v>21001.126832864611</v>
       </c>
       <c r="X102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.4964191886164116</v>
       </c>
       <c r="Y102">
         <v>20852.16905141146</v>
       </c>
       <c r="Z102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.60114017464335112</v>
       </c>
       <c r="AA102">
@@ -9257,7 +9217,7 @@
         <v>118.73284099999999</v>
       </c>
       <c r="F103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.11562597922072529</v>
       </c>
       <c r="G103">
@@ -9312,14 +9272,14 @@
         <v>20821.876063758969</v>
       </c>
       <c r="X103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.41152640995841178</v>
       </c>
       <c r="Y103">
         <v>20679.116488082691</v>
       </c>
       <c r="Z103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.51902157583788644</v>
       </c>
       <c r="AA103">
@@ -9350,7 +9310,7 @@
         <v>119.60525</v>
       </c>
       <c r="F104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.10770189757028192</v>
       </c>
       <c r="G104">
@@ -9405,14 +9365,14 @@
         <v>20316.78793364004</v>
       </c>
       <c r="X104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.2790910453690113</v>
       </c>
       <c r="Y104">
         <v>20248.772524617441</v>
       </c>
       <c r="Z104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.38351890039902942</v>
       </c>
       <c r="AA104">
@@ -9443,7 +9403,7 @@
         <v>120.42763600000001</v>
       </c>
       <c r="F105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.9509468365643464E-2</v>
       </c>
       <c r="G105">
@@ -9498,14 +9458,14 @@
         <v>19788.088757301521</v>
       </c>
       <c r="X105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.17242743971881777</v>
       </c>
       <c r="Y105">
         <v>19793.239153179089</v>
       </c>
       <c r="Z105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.26984855931223994</v>
       </c>
       <c r="AA105">
@@ -9536,7 +9496,7 @@
         <v>121.189266</v>
       </c>
       <c r="F106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.1572065958517759E-2</v>
       </c>
       <c r="G106">
@@ -9591,14 +9551,14 @@
         <v>19706.048058744738</v>
       </c>
       <c r="X106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.21793098219842874</v>
       </c>
       <c r="Y106">
         <v>19753.050983904799</v>
       </c>
       <c r="Z106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.29269450433526167</v>
       </c>
       <c r="AA106">
@@ -9629,7 +9589,7 @@
         <v>121.883482</v>
       </c>
       <c r="F107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.4243750780545579E-2</v>
       </c>
       <c r="G107">
@@ -9684,14 +9644,14 @@
         <v>20046.243838028851</v>
       </c>
       <c r="X107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.21079618729901897</v>
       </c>
       <c r="Y107">
         <v>20254.3442268904</v>
       </c>
       <c r="Z107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.28220004075025068</v>
       </c>
       <c r="AA107">
@@ -9722,7 +9682,7 @@
         <v>122.509117</v>
       </c>
       <c r="F108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.7674074932500184E-2</v>
       </c>
       <c r="G108">
@@ -9777,14 +9737,14 @@
         <v>21311.899587032371</v>
       </c>
       <c r="X108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.22428537425574963</v>
       </c>
       <c r="Y108">
         <v>21946.009536580041</v>
       </c>
       <c r="Z108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.31644889768937412</v>
       </c>
       <c r="AA108">
@@ -9815,7 +9775,7 @@
         <v>123.07271</v>
       </c>
       <c r="F109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.180208714556241E-2</v>
       </c>
       <c r="G109">
@@ -9870,14 +9830,14 @@
         <v>22579.983409807101</v>
       </c>
       <c r="X109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.2286865203733135</v>
       </c>
       <c r="Y109">
         <v>23362.333940643701</v>
       </c>
       <c r="Z109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.32495745240942708</v>
       </c>
       <c r="AA109">
@@ -9908,7 +9868,7 @@
         <v>123.58452699999999</v>
       </c>
       <c r="F110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.6494377494510176E-2</v>
       </c>
       <c r="G110">
@@ -9963,14 +9923,14 @@
         <v>24743.18649939082</v>
       </c>
       <c r="X110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.25375904327027088</v>
       </c>
       <c r="Y110">
         <v>25594.397428085798</v>
       </c>
       <c r="Z110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.36208744572292839</v>
       </c>
       <c r="AA110">
@@ -10001,7 +9961,7 @@
         <v>124.05852</v>
       </c>
       <c r="F111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.1532700371864327E-2</v>
       </c>
       <c r="G111">
@@ -10056,14 +10016,14 @@
         <v>26602.838321785559</v>
       </c>
       <c r="X111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.28962965156188247</v>
       </c>
       <c r="Y111">
         <v>27335.0310804933</v>
       </c>
       <c r="Z111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.37544308098043905</v>
       </c>
       <c r="AA111">
@@ -10094,7 +10054,7 @@
         <v>124.50524</v>
       </c>
       <c r="F112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.6768576742869045E-2</v>
       </c>
       <c r="G112">
@@ -10149,14 +10109,14 @@
         <v>28533.84524217615</v>
       </c>
       <c r="X112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.35868163024107863</v>
       </c>
       <c r="Y112">
         <v>29385.457993575212</v>
       </c>
       <c r="Z112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.4092278803766049</v>
       </c>
       <c r="AA112">
@@ -10187,7 +10147,7 @@
         <v>124.929772</v>
       </c>
       <c r="F113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5.2192223716772741E-2</v>
       </c>
       <c r="G113">
@@ -10242,14 +10202,14 @@
         <v>30171.953327506271</v>
       </c>
       <c r="X113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.44905066359612816</v>
       </c>
       <c r="Y113">
         <v>31110.08639317776</v>
       </c>
       <c r="Z113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.50442048194401368</v>
       </c>
       <c r="AA113">
@@ -10280,7 +10240,7 @@
         <v>125.33129700000001</v>
       </c>
       <c r="F114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.7874545640764168E-2</v>
       </c>
       <c r="G114">
@@ -10335,14 +10295,14 @@
         <v>31104.29791530842</v>
       </c>
       <c r="X114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.53096532861903256</v>
       </c>
       <c r="Y114">
         <v>32143.32609994453</v>
       </c>
       <c r="Z114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.587420968894104</v>
       </c>
       <c r="AA114">
@@ -10373,7 +10333,7 @@
         <v>125.70741099999999</v>
       </c>
       <c r="F115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.3841888584444072E-2</v>
       </c>
       <c r="G115">
@@ -10428,14 +10388,14 @@
         <v>31836.17392295193</v>
       </c>
       <c r="X115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.60885542375611379</v>
       </c>
       <c r="Y115">
         <v>33009.440071914301</v>
       </c>
       <c r="Z115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.66771289006592405</v>
       </c>
       <c r="AA115">
@@ -10466,7 +10426,7 @@
         <v>126.053129</v>
       </c>
       <c r="F116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.0134437318895842E-2</v>
       </c>
       <c r="G116">
@@ -10521,14 +10481,14 @@
         <v>32890.355700729968</v>
       </c>
       <c r="X116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.66904879165432529</v>
       </c>
       <c r="Y116">
         <v>33976.026886250482</v>
       </c>
       <c r="Z116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.72003944676368536</v>
       </c>
       <c r="AA116">
@@ -10559,7 +10519,7 @@
         <v>126.365484</v>
       </c>
       <c r="F117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.6772841786715561E-2</v>
       </c>
       <c r="G117">
@@ -10614,14 +10574,14 @@
         <v>34702.830719185949</v>
       </c>
       <c r="X117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.73113881082064502</v>
       </c>
       <c r="Y117">
         <v>35783.742972091968</v>
       </c>
       <c r="Z117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.76671940455046561</v>
       </c>
       <c r="AA117">
@@ -10652,7 +10612,7 @@
         <v>126.644094</v>
       </c>
       <c r="F118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.3752402280395118E-2</v>
       </c>
       <c r="G118">
@@ -10707,14 +10667,14 @@
         <v>36720.480625018332</v>
       </c>
       <c r="X118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.72300364287384333</v>
       </c>
       <c r="Y118">
         <v>37559.607793475152</v>
       </c>
       <c r="Z118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.71145500191595457</v>
       </c>
       <c r="AA118">
@@ -10745,7 +10705,7 @@
         <v>126.89273799999999</v>
       </c>
       <c r="F119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.1038789996580017E-2</v>
       </c>
       <c r="G119">
@@ -10800,14 +10760,14 @@
         <v>36845.118749033543</v>
       </c>
       <c r="X119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.63176022233172713</v>
       </c>
       <c r="Y119">
         <v>37646.122034186068</v>
       </c>
       <c r="Z119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.61140244505677188</v>
       </c>
       <c r="AA119">
@@ -10838,7 +10798,7 @@
         <v>127.117434</v>
       </c>
       <c r="F120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.8586968658301445E-2</v>
       </c>
       <c r="G120">
@@ -10893,14 +10853,14 @@
         <v>36408.223910498382</v>
       </c>
       <c r="X120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.47144442820227522</v>
       </c>
       <c r="Y120">
         <v>37128.616834729379</v>
       </c>
       <c r="Z120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.45065407142528002</v>
       </c>
       <c r="AA120">
@@ -10931,7 +10891,7 @@
         <v>127.32607</v>
       </c>
       <c r="F121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.6338779472784294E-2</v>
       </c>
       <c r="G121">
@@ -10986,14 +10946,14 @@
         <v>36082.382814454257</v>
       </c>
       <c r="X121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.35633583071118102</v>
       </c>
       <c r="Y121">
         <v>37066.07766971839</v>
       </c>
       <c r="Z121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.35599178799431896</v>
       </c>
       <c r="AA121">
@@ -11024,7 +10984,7 @@
         <v>127.524174</v>
       </c>
       <c r="F122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.4247445328405469E-2</v>
       </c>
       <c r="G122">
@@ -11079,14 +11039,14 @@
         <v>36829.648471198881</v>
       </c>
       <c r="X122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.29073555136412615</v>
       </c>
       <c r="Y122">
         <v>37915.274009145913</v>
       </c>
       <c r="Z122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.2902733732254793</v>
       </c>
       <c r="AA122">
@@ -11117,7 +11077,7 @@
         <v>127.71382800000001</v>
       </c>
       <c r="F123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.22849682299909E-2</v>
       </c>
       <c r="G123">
@@ -11172,14 +11132,14 @@
         <v>36889.126054541252</v>
       </c>
       <c r="X123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.2226296936801658</v>
       </c>
       <c r="Y123">
         <v>37468.683500740422</v>
       </c>
       <c r="Z123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.20439021053175413</v>
       </c>
       <c r="AA123">
@@ -11210,7 +11170,7 @@
         <v>127.893078</v>
       </c>
       <c r="F124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.0440074118119086E-2</v>
       </c>
       <c r="G124">
@@ -11265,14 +11225,14 @@
         <v>36764.648044517307</v>
       </c>
       <c r="X124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.1819796783268034</v>
       </c>
       <c r="Y124">
         <v>37384.548677450708</v>
       </c>
       <c r="Z124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.16305787898892091</v>
       </c>
       <c r="AA124">
@@ -11303,7 +11263,7 @@
         <v>128.05837199999999</v>
       </c>
       <c r="F125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.8701848851218471E-2</v>
       </c>
       <c r="G125">
@@ -11358,14 +11318,14 @@
         <v>37266.665392247844</v>
       </c>
       <c r="X125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.17057613400525062</v>
       </c>
       <c r="Y125">
         <v>37952.087193487037</v>
       </c>
       <c r="Z125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.14973435207639677</v>
       </c>
       <c r="AA125">
@@ -11396,7 +11356,7 @@
         <v>128.204195</v>
       </c>
       <c r="F126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.7064756877237058E-2</v>
       </c>
       <c r="G126">
@@ -11451,14 +11411,14 @@
         <v>37997.863486448317</v>
       </c>
       <c r="X126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.15528891910417963</v>
       </c>
       <c r="Y126">
         <v>38901.745765807427</v>
       </c>
       <c r="Z126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.14497630626582475</v>
       </c>
       <c r="AA126">
@@ -11489,7 +11449,7 @@
         <v>128.32611600000001</v>
       </c>
       <c r="F127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.5515565943624434E-2</v>
       </c>
       <c r="G127">
@@ -11544,14 +11504,14 @@
         <v>38466.328241400217</v>
       </c>
       <c r="X127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.10844929489090828</v>
       </c>
       <c r="Y127">
         <v>39823.616262180018</v>
       </c>
       <c r="Z127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.11289688988764478</v>
       </c>
       <c r="AA127">
@@ -11582,7 +11542,7 @@
         <v>128.42273399999999</v>
       </c>
       <c r="F128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.4044397522398446E-2</v>
       </c>
       <c r="G128">
@@ -11637,14 +11597,14 @@
         <v>38982.743507080297</v>
       </c>
       <c r="X128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.1607659909566757E-2</v>
       </c>
       <c r="Y128">
         <v>40255.95655049674</v>
       </c>
       <c r="Z128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.1788522708961744E-2</v>
       </c>
       <c r="AA128">
@@ -11675,7 +11635,7 @@
         <v>128.494057</v>
       </c>
       <c r="F129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2619469208710776E-2</v>
       </c>
       <c r="G129">
@@ -11730,14 +11690,14 @@
         <v>39759.03726037695</v>
       </c>
       <c r="X129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.9085605102571149E-2</v>
       </c>
       <c r="Y129">
         <v>41021.091738118288</v>
       </c>
       <c r="Z129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9649863560115006E-2</v>
       </c>
       <c r="AA129">
@@ -11768,7 +11728,7 @@
         <v>128.538646</v>
       </c>
       <c r="F130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.1180307494249742E-2</v>
       </c>
       <c r="G130">
@@ -11823,14 +11783,14 @@
         <v>39038.768931796592</v>
       </c>
       <c r="X130">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.2251396491211095E-2</v>
       </c>
       <c r="Y130">
         <v>40303.450839212979</v>
       </c>
       <c r="Z130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.5509083697239238E-2</v>
       </c>
       <c r="AA130">
@@ -11861,7 +11821,7 @@
         <v>128.55518900000001</v>
       </c>
       <c r="F131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.6533176591409083E-3</v>
       </c>
       <c r="G131">
@@ -11916,14 +11876,14 @@
         <v>37378.852906513173</v>
       </c>
       <c r="X131">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.5930833579526325E-2</v>
       </c>
       <c r="Y131">
         <v>38058.358733384157</v>
       </c>
       <c r="Z131">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.6770597971212468E-2</v>
       </c>
       <c r="AA131">
@@ -11954,7 +11914,7 @@
         <v>128.54235299999999</v>
       </c>
       <c r="F132">
-        <f t="shared" si="3"/>
+        <f>(E132-E122)/E122</f>
         <v>7.9842038420102936E-3</v>
       </c>
       <c r="G132">
@@ -12009,14 +11969,14 @@
         <v>38652.015340033497</v>
       </c>
       <c r="X132">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.9480973739397013E-2</v>
       </c>
       <c r="Y132">
         <v>39789.702620427372</v>
       </c>
       <c r="Z132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.943729566161937E-2</v>
       </c>
       <c r="AA132">
@@ -12047,7 +12007,7 @@
         <v>128.498965</v>
       </c>
       <c r="F133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.1476271778494627E-3</v>
       </c>
       <c r="G133">
@@ -12102,14 +12062,14 @@
         <v>38203.381638132261</v>
       </c>
       <c r="X133">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.5627181344655839E-2</v>
       </c>
       <c r="Y133">
         <v>39162.327105124932</v>
       </c>
       <c r="Z133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.5201577588148821E-2</v>
       </c>
       <c r="AA133">
@@ -12140,7 +12100,7 @@
         <v>128.42357100000001</v>
       </c>
       <c r="F134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.1479414546579836E-3</v>
       </c>
       <c r="G134">
@@ -12195,14 +12155,14 @@
         <v>38687.064697803813</v>
       </c>
       <c r="X134">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.2289815231161843E-2</v>
       </c>
       <c r="Y134">
         <v>39235.846354093374</v>
       </c>
       <c r="Z134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.9520396584573863E-2</v>
       </c>
       <c r="AA134">
@@ -12233,7 +12193,7 @@
         <v>128.31419500000001</v>
       </c>
       <c r="F135">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.9977061710578421E-3</v>
       </c>
       <c r="G135">
@@ -12288,14 +12248,14 @@
         <v>39305.230415076061</v>
       </c>
       <c r="X135">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>5.4702104451027078E-2</v>
       </c>
       <c r="Y135">
         <v>39666.531049039433</v>
       </c>
       <c r="Z135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.5173901683241591E-2</v>
       </c>
       <c r="AA135">
@@ -12326,7 +12286,7 @@
         <v>128.16863900000001</v>
       </c>
       <c r="F136">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.7733881874914847E-4</v>
       </c>
       <c r="G136">
@@ -12381,14 +12341,14 @@
         <v>38724.847503452067</v>
       </c>
       <c r="X136">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.913223403371149E-2</v>
       </c>
       <c r="Y136">
         <v>39171.81331698467</v>
       </c>
       <c r="Z136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.9422990115424969E-3</v>
       </c>
       <c r="AA136">
@@ -12419,7 +12379,7 @@
         <v>127.985133</v>
       </c>
       <c r="F137">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-2.6571598255183569E-3</v>
       </c>
       <c r="G137">
@@ -12474,14 +12434,14 @@
         <v>39804.904527465696</v>
       </c>
       <c r="X137">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.4798649813028111E-2</v>
       </c>
       <c r="Y137">
         <v>40274.205129747381</v>
       </c>
       <c r="Z137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.1314614539294908E-2</v>
       </c>
       <c r="AA137">
@@ -12512,7 +12472,7 @@
         <v>127.763265</v>
       </c>
       <c r="F138">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-5.1351421937488673E-3</v>
       </c>
       <c r="G138">
@@ -12567,14 +12527,14 @@
         <v>38999.320344545049</v>
       </c>
       <c r="X138">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.2523527010718281E-4</v>
       </c>
       <c r="Y138">
         <v>39467.091734075519</v>
       </c>
       <c r="Z138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-1.9596225851239563E-2</v>
       </c>
       <c r="AA138">
@@ -12605,7 +12565,7 @@
         <v>127.502725</v>
       </c>
       <c r="F139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.7150027257680866E-3</v>
       </c>
       <c r="G139">
@@ -12660,14 +12620,14 @@
         <v>39241.259353476562</v>
       </c>
       <c r="X139">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-1.3022898505049948E-2</v>
       </c>
       <c r="Y139">
         <v>39598.290938487793</v>
       </c>
       <c r="Z139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-3.4684615629290455E-2</v>
       </c>
       <c r="AA139">
@@ -12698,7 +12658,7 @@
         <v>127.202192</v>
       </c>
       <c r="F140">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.0397293277852042E-2</v>
       </c>
       <c r="G140">
@@ -12753,14 +12713,14 @@
         <v>39175.983696884723</v>
       </c>
       <c r="X140">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.5148333014254182E-3</v>
       </c>
       <c r="Y140">
         <v>39352.128460176224</v>
       </c>
       <c r="Z140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-2.360399318738168E-2</v>
       </c>
       <c r="AA140">
@@ -12885,10 +12845,6 @@
       <c r="E142">
         <v>155.58397296844001</v>
       </c>
-      <c r="F142">
-        <f t="shared" si="6"/>
-        <v>0.21037128492925611</v>
-      </c>
       <c r="G142">
         <v>2.5832128524780269</v>
       </c>
@@ -12898,16 +12854,8 @@
       <c r="W142">
         <v>15733.91817482744</v>
       </c>
-      <c r="X142">
-        <f t="shared" si="7"/>
-        <v>-0.59293408024364591</v>
-      </c>
       <c r="Y142">
         <v>15911.84138550169</v>
-      </c>
-      <c r="Z142">
-        <f t="shared" si="8"/>
-        <v>-0.60010152532950023</v>
       </c>
     </row>
     <row r="143" spans="1:30" x14ac:dyDescent="0.35">
@@ -12924,10 +12872,6 @@
       <c r="E143">
         <v>158.24770385810939</v>
       </c>
-      <c r="F143">
-        <f t="shared" si="6"/>
-        <v>0.23150956008174378</v>
-      </c>
       <c r="G143">
         <v>2.595999956130981</v>
       </c>
@@ -12949,16 +12893,8 @@
       <c r="W143">
         <v>16560.23080341021</v>
       </c>
-      <c r="X143">
-        <f t="shared" si="7"/>
-        <v>-0.56652447785196036</v>
-      </c>
       <c r="Y143">
         <v>16814.245547510651</v>
-      </c>
-      <c r="Z143">
-        <f t="shared" si="8"/>
-        <v>-0.57065254313474456</v>
       </c>
       <c r="AA143">
         <v>5.2517918257943913E-2</v>
@@ -12981,10 +12917,6 @@
       <c r="E144">
         <v>160.98089165584281</v>
       </c>
-      <c r="F144">
-        <f t="shared" si="6"/>
-        <v>0.25351514836667172</v>
-      </c>
       <c r="G144">
         <v>2.608850240707397</v>
       </c>
@@ -13006,16 +12938,8 @@
       <c r="W144">
         <v>16890.197165840538</v>
       </c>
-      <c r="X144">
-        <f t="shared" si="7"/>
-        <v>-0.56341487011808988</v>
-      </c>
       <c r="Y144">
         <v>17094.78355905303</v>
-      </c>
-      <c r="Z144">
-        <f t="shared" si="8"/>
-        <v>-0.56430700118516552</v>
       </c>
       <c r="AA144">
         <v>1.9925227271734819E-2</v>
@@ -13038,10 +12962,6 @@
       <c r="E145">
         <v>163.66914683650771</v>
       </c>
-      <c r="F145">
-        <f t="shared" si="6"/>
-        <v>0.27553422157624641</v>
-      </c>
       <c r="G145">
         <v>2.6217644214630131</v>
       </c>
@@ -13063,16 +12983,8 @@
       <c r="W145">
         <v>17429.46398351782</v>
       </c>
-      <c r="X145">
-        <f t="shared" si="7"/>
-        <v>-0.55656120573631063</v>
-      </c>
       <c r="Y145">
         <v>17586.408652054892</v>
-      </c>
-      <c r="Z145">
-        <f t="shared" si="8"/>
-        <v>-0.55664364422709545</v>
       </c>
       <c r="AA145">
         <v>3.1927798851745487E-2</v>
@@ -13095,10 +13007,6 @@
       <c r="E146">
         <v>166.57297567997881</v>
       </c>
-      <c r="F146">
-        <f t="shared" si="6"/>
-        <v>0.2996391081283058</v>
-      </c>
       <c r="G146">
         <v>2.6347424983978271</v>
       </c>
@@ -13126,16 +13034,8 @@
       <c r="W146">
         <v>17039.06944337035</v>
       </c>
-      <c r="X146">
-        <f t="shared" si="7"/>
-        <v>-0.55999647405063557</v>
-      </c>
       <c r="Y146">
         <v>17226.949559411059</v>
-      </c>
-      <c r="Z146">
-        <f t="shared" si="8"/>
-        <v>-0.56022077865000053</v>
       </c>
       <c r="AA146">
         <v>-2.239853965197364E-2</v>
@@ -13158,10 +13058,6 @@
       <c r="E147">
         <v>169.5411788384661</v>
       </c>
-      <c r="F147">
-        <f t="shared" si="6"/>
-        <v>0.32469432085104827</v>
-      </c>
       <c r="G147">
         <v>2.6477844715118408</v>
       </c>
@@ -13195,16 +13091,8 @@
       <c r="W147">
         <v>18016.987205865509</v>
       </c>
-      <c r="X147">
-        <f t="shared" si="7"/>
-        <v>-0.54736765683149302</v>
-      </c>
       <c r="Y147">
         <v>18205.358846423871</v>
-      </c>
-      <c r="Z147">
-        <f t="shared" si="8"/>
-        <v>-0.5479647881870422</v>
       </c>
       <c r="AA147">
         <v>5.7392674273984409E-2</v>
@@ -13227,10 +13115,6 @@
       <c r="E148">
         <v>172.57784109533941</v>
       </c>
-      <c r="F148">
-        <f t="shared" si="6"/>
-        <v>0.35076260844883234</v>
-      </c>
       <c r="G148">
         <v>2.662317276000977</v>
       </c>
@@ -13264,16 +13148,8 @@
       <c r="W148">
         <v>18098.39681720499</v>
       </c>
-      <c r="X148">
-        <f t="shared" si="7"/>
-        <v>-0.53593045577943088</v>
-      </c>
       <c r="Y148">
         <v>18296.603028285728</v>
-      </c>
-      <c r="Z148">
-        <f t="shared" si="8"/>
-        <v>-0.53640863249904447</v>
       </c>
       <c r="AA148">
         <v>4.5184919326015172E-3</v>
@@ -13296,10 +13172,6 @@
       <c r="E149">
         <v>175.72586826675851</v>
       </c>
-      <c r="F149">
-        <f t="shared" si="6"/>
-        <v>0.37821264813562622</v>
-      </c>
       <c r="G149">
         <v>2.6769299507141109</v>
       </c>
@@ -13333,16 +13205,8 @@
       <c r="W149">
         <v>18164.218117019289</v>
       </c>
-      <c r="X149">
-        <f t="shared" si="7"/>
-        <v>-0.53711429204144445</v>
-      </c>
       <c r="Y149">
         <v>18360.442784110732</v>
-      </c>
-      <c r="Z149">
-        <f t="shared" si="8"/>
-        <v>-0.53633244392713952</v>
       </c>
       <c r="AA149">
         <v>3.636858031078178E-3</v>
@@ -13365,10 +13229,6 @@
       <c r="E150">
         <v>178.68693084973671</v>
       </c>
-      <c r="F150">
-        <f t="shared" si="6"/>
-        <v>0.40474726135015593</v>
-      </c>
       <c r="G150">
         <v>2.6916227340698242</v>
       </c>
@@ -13402,16 +13262,8 @@
       <c r="W150">
         <v>17741.52835310547</v>
       </c>
-      <c r="X150">
-        <f t="shared" si="7"/>
-        <v>-0.54713253685276886</v>
-      </c>
       <c r="Y150">
         <v>17873.422442325791</v>
-      </c>
-      <c r="Z150">
-        <f t="shared" si="8"/>
-        <v>-0.54580798697042698</v>
       </c>
       <c r="AA150">
         <v>-2.327046290628763E-2</v>
@@ -13434,10 +13286,6 @@
       <c r="E151">
         <v>181.69906881561451</v>
       </c>
-      <c r="F151">
-        <f t="shared" si="6"/>
-        <v>0.43227682248376897</v>
-      </c>
       <c r="G151">
         <v>2.706396102905273</v>
       </c>
@@ -13471,16 +13319,8 @@
       <c r="W151">
         <v>18713.42281588952</v>
       </c>
-      <c r="X151">
-        <f t="shared" si="7"/>
-        <v>-0.52787864897894665</v>
-      </c>
       <c r="Y151">
         <v>18855.439228897041</v>
-      </c>
-      <c r="Z151">
-        <f t="shared" si="8"/>
-        <v>-0.52510254915877941</v>
       </c>
       <c r="AA151">
         <v>5.4780763158655953E-2</v>
@@ -13552,10 +13392,6 @@
       <c r="W152">
         <v>18900.7482995768</v>
       </c>
-      <c r="X152">
-        <f t="shared" si="7"/>
-        <v>0.20127409393903828</v>
-      </c>
       <c r="Y152">
         <v>19079.52491462891</v>
       </c>
@@ -15395,7 +15231,7 @@
         <v>30788.47069358615</v>
       </c>
       <c r="X172">
-        <f t="shared" si="7"/>
+        <f>(W172-W162)/W162</f>
         <v>0.21436080851152992</v>
       </c>
       <c r="Y172">

</xml_diff>